<commit_message>
Visão e Escopo, Requisitos, Cronograma
</commit_message>
<xml_diff>
--- a/docs/Sprints Backlogs/Sprint1 Backlog.xlsx
+++ b/docs/Sprints Backlogs/Sprint1 Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="15405" windowHeight="6270" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="15405" windowHeight="6270"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint #2" sheetId="6" r:id="rId1"/>
@@ -1014,7 +1014,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -1184,6 +1184,9 @@
   </si>
   <si>
     <t>eBM</t>
+  </si>
+  <si>
+    <t>Todos</t>
   </si>
 </sst>
 </file>
@@ -1530,6 +1533,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1547,9 +1553,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1669,7 +1672,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.1704857107406077"/>
-          <c:y val="2.6881786835469133E-2"/>
+          <c:y val="2.6881786835469143E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -1792,11 +1795,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="90875392"/>
-        <c:axId val="90877312"/>
+        <c:axId val="81117952"/>
+        <c:axId val="81119872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="90875392"/>
+        <c:axId val="81117952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1828,7 +1831,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.41558653408557089"/>
+              <c:x val="0.41558653408557095"/>
               <c:y val="0.93052333586002856"/>
             </c:manualLayout>
           </c:layout>
@@ -1866,7 +1869,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90877312"/>
+        <c:crossAx val="81119872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1875,7 +1878,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90877312"/>
+        <c:axId val="81119872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1957,7 +1960,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90875392"/>
+        <c:crossAx val="81117952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2372,11 +2375,11 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:BA42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X22" sqref="X22"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2409,11 +2412,11 @@
       <c r="B1" s="36"/>
       <c r="N1" s="38"/>
       <c r="P1" s="38"/>
-      <c r="Q1" s="65" t="s">
+      <c r="Q1" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="66"/>
-      <c r="S1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="68"/>
     </row>
     <row r="2" spans="1:53" s="15" customFormat="1" ht="40.5" customHeight="1">
       <c r="A2" s="35" t="s">
@@ -2533,15 +2536,15 @@
       </c>
       <c r="B3" s="44"/>
       <c r="C3" s="28"/>
-      <c r="D3" s="71">
+      <c r="D3" s="65">
         <v>41568</v>
       </c>
-      <c r="E3" s="71">
+      <c r="E3" s="65">
         <v>41575</v>
       </c>
       <c r="F3" s="59"/>
       <c r="G3" s="60" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H3" s="60">
         <v>9</v>
@@ -3086,7 +3089,7 @@
         <v>2.5</v>
       </c>
       <c r="X22">
-        <f t="shared" ref="X22:AP22" si="6">W22+X21</f>
+        <f t="shared" ref="X22:Z22" si="6">W22+X21</f>
         <v>4</v>
       </c>
       <c r="Y22">
@@ -3145,7 +3148,7 @@
         <v>1</v>
       </c>
       <c r="U24" s="11">
-        <f t="shared" ref="U24:AP24" ca="1" si="7">IF(U2 &lt; $S$30, U23/$O$21, NA())</f>
+        <f t="shared" ref="U24:Z24" ca="1" si="7">IF(U2 &lt; $S$30, U23/$O$21, NA())</f>
         <v>0.83333333333333337</v>
       </c>
       <c r="V24" s="11">
@@ -3333,7 +3336,7 @@
       </c>
       <c r="S30" s="39">
         <f ca="1">NOW()</f>
-        <v>41675.826051041666</v>
+        <v>41688.93304236111</v>
       </c>
     </row>
     <row r="32" spans="1:53">
@@ -3411,7 +3414,7 @@
   <sheetPr codeName="Plan2"/>
   <dimension ref="P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
@@ -3440,7 +3443,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3556,7 +3559,9 @@
         <v>6</v>
       </c>
       <c r="D7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="F7" s="41" t="s">
+        <v>55</v>
+      </c>
       <c r="I7">
         <v>36</v>
       </c>
@@ -3659,11 +3664,11 @@
     <row r="1" spans="1:51" s="21" customFormat="1">
       <c r="K1" s="33"/>
       <c r="L1" s="17"/>
-      <c r="O1" s="68" t="s">
+      <c r="O1" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="71"/>
     </row>
     <row r="2" spans="1:51" s="15" customFormat="1" ht="40.5" customHeight="1">
       <c r="A2" s="15" t="s">

</xml_diff>